<commit_message>
Update results of 003
</commit_message>
<xml_diff>
--- a/20160408 - 003/running_logs/logs.xlsx
+++ b/20160408 - 003/running_logs/logs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="61">
   <si>
     <t>Time</t>
   </si>
@@ -176,6 +176,27 @@
   </si>
   <si>
     <t>20160409_093805</t>
+  </si>
+  <si>
+    <t>20160411_112803</t>
+  </si>
+  <si>
+    <t>convert to lower, trim "space" and ",", convert unicode to ascii, remove multiple spaces</t>
+  </si>
+  <si>
+    <t>2 layers: [100-Sigmoid, 3-Softmax], learning_rate: 0.01, learning_rule: adagrad, n_iterator: 2000</t>
+  </si>
+  <si>
+    <t>20160411_114521</t>
+  </si>
+  <si>
+    <t>20160411_120318</t>
+  </si>
+  <si>
+    <t>20160411_122151</t>
+  </si>
+  <si>
+    <t>20160411_124110</t>
   </si>
 </sst>
 </file>
@@ -507,7 +528,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1502,6 +1523,166 @@
         <v>0.195876288659794</v>
       </c>
     </row>
+    <row r="32" spans="1:10">
+      <c r="A32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32">
+        <v>1038.199</v>
+      </c>
+      <c r="C32" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" t="s">
+        <v>56</v>
+      </c>
+      <c r="G32">
+        <v>0.973333333333333</v>
+      </c>
+      <c r="H32">
+        <v>0.993399339933993</v>
+      </c>
+      <c r="I32" t="s">
+        <v>14</v>
+      </c>
+      <c r="J32">
+        <v>0.175257731958763</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33">
+        <v>1076.55</v>
+      </c>
+      <c r="C33" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" t="s">
+        <v>56</v>
+      </c>
+      <c r="G33">
+        <v>0.980666666666667</v>
+      </c>
+      <c r="H33">
+        <v>0.986798679867987</v>
+      </c>
+      <c r="I33" t="s">
+        <v>14</v>
+      </c>
+      <c r="J33">
+        <v>0.157894736842105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34">
+        <v>1113.259</v>
+      </c>
+      <c r="C34" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" t="s">
+        <v>56</v>
+      </c>
+      <c r="G34">
+        <v>0.980666666666667</v>
+      </c>
+      <c r="H34">
+        <v>0.986798679867987</v>
+      </c>
+      <c r="I34" t="s">
+        <v>14</v>
+      </c>
+      <c r="J34">
+        <v>0.157894736842105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35">
+        <v>1159.053</v>
+      </c>
+      <c r="C35" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" t="s">
+        <v>56</v>
+      </c>
+      <c r="G35">
+        <v>0.982</v>
+      </c>
+      <c r="H35">
+        <v>0.986798679867987</v>
+      </c>
+      <c r="I35" t="s">
+        <v>14</v>
+      </c>
+      <c r="J35">
+        <v>0.168421052631579</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36">
+        <v>1162.679</v>
+      </c>
+      <c r="C36" t="s">
+        <v>55</v>
+      </c>
+      <c r="D36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" t="s">
+        <v>56</v>
+      </c>
+      <c r="G36">
+        <v>0.979333333333333</v>
+      </c>
+      <c r="H36">
+        <v>0.993399339933993</v>
+      </c>
+      <c r="I36" t="s">
+        <v>14</v>
+      </c>
+      <c r="J36">
+        <v>0.154639175257732</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>